<commit_message>
[WBCAMS-1548] Fix typo in top 10 occupations dataset
</commit_message>
<xml_diff>
--- a/migration/data/top_10_careers_by_aggregate_industry_2025.xlsx
+++ b/migration/data/top_10_careers_by_aggregate_industry_2025.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="312">
   <si>
     <t xml:space="preserve">Aggregate Industry</t>
   </si>
@@ -125,7 +133,7 @@
     <t xml:space="preserve">#00018</t>
   </si>
   <si>
-    <t xml:space="preserve">Seniors managers - public and private sector</t>
+    <t xml:space="preserve">Senior managers - public and private sector</t>
   </si>
   <si>
     <t xml:space="preserve">#83120</t>
@@ -953,15 +961,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -973,7 +998,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -981,2840 +1006,2605 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17 C30 C61 C97 C109 C116 C130 C136 C178"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="86.88"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="0" t="n">
         <v>9290</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="0" t="n">
         <v>8210</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="0" t="n">
         <v>6000</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="0" t="n">
         <v>4040</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="0" t="n">
         <v>3660</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="0" t="n">
         <v>2690</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="0" t="n">
         <v>2460</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="0" t="n">
         <v>2310</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="0" t="n">
         <v>1390</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" s="0" t="n">
         <v>840</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" s="0" t="n">
         <v>790</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" s="0" t="n">
         <v>120</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="0" t="n">
         <v>90</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" s="0" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" s="0" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" s="0" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" s="0" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" s="0" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" s="0" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" s="0" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" s="0" t="n">
         <v>4530</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" s="0" t="n">
         <v>2920</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" s="0" t="n">
         <v>2670</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" s="0" t="n">
         <v>2320</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="s">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" s="0" t="n">
         <v>1140</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="s">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" s="0" t="n">
         <v>910</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="s">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" s="0" t="n">
         <v>830</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="s">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29" s="0" t="n">
         <v>770</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="s">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30" s="0" t="n">
         <v>710</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="s">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31" s="0" t="n">
         <v>690</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="s">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32" s="0" t="n">
         <v>9260</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="s">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33" s="0" t="n">
         <v>8530</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="s">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34" s="0" t="n">
         <v>7440</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="s">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35" s="0" t="n">
         <v>6380</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="s">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36" s="0" t="n">
         <v>3760</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="s">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37" s="0" t="n">
         <v>3360</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="s">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38" s="0" t="n">
         <v>2680</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="s">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39" s="0" t="n">
         <v>2530</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="s">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40" s="0" t="n">
         <v>2120</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="s">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41" s="0" t="n">
         <v>2050</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="s">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42" s="0" t="n">
         <v>9470</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="s">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43" s="0" t="n">
         <v>5370</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="s">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D44" s="0" t="n">
         <v>5160</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="s">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D45" s="0" t="n">
         <v>4200</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="s">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="D46" t="n">
+      <c r="D46" s="0" t="n">
         <v>3010</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="s">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D47" t="n">
+      <c r="D47" s="0" t="n">
         <v>2290</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="s">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48" s="0" t="n">
         <v>2250</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="s">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D49" s="0" t="n">
         <v>1790</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="s">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50" s="0" t="n">
         <v>1750</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="s">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D51" s="0" t="n">
         <v>1620</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="s">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="D52" t="n">
+      <c r="D52" s="0" t="n">
         <v>6890</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="s">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="D53" t="n">
+      <c r="D53" s="0" t="n">
         <v>4800</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="s">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="D54" t="n">
+      <c r="D54" s="0" t="n">
         <v>4610</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="s">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D55" t="n">
+      <c r="D55" s="0" t="n">
         <v>3980</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="s">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="D56" t="n">
+      <c r="D56" s="0" t="n">
         <v>3720</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="s">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="D57" t="n">
+      <c r="D57" s="0" t="n">
         <v>3560</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="s">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="D58" t="n">
+      <c r="D58" s="0" t="n">
         <v>2690</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="s">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="D59" t="n">
+      <c r="D59" s="0" t="n">
         <v>2250</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="s">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="D60" t="n">
+      <c r="D60" s="0" t="n">
         <v>2110</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="s">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D61" t="n">
+      <c r="D61" s="0" t="n">
         <v>2040</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="s">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="D62" t="n">
+      <c r="D62" s="0" t="n">
         <v>470</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="s">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D63" t="n">
+      <c r="D63" s="0" t="n">
         <v>420</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="s">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="D64" t="n">
+      <c r="D64" s="0" t="n">
         <v>370</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="s">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="D65" t="n">
+      <c r="D65" s="0" t="n">
         <v>330</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" t="s">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="D66" t="n">
+      <c r="D66" s="0" t="n">
         <v>330</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" t="s">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="D67" t="n">
+      <c r="D67" s="0" t="n">
         <v>310</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="s">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="D68" t="n">
+      <c r="D68" s="0" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" t="s">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="D69" t="n">
+      <c r="D69" s="0" t="n">
         <v>140</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="s">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="D70" t="n">
+      <c r="D70" s="0" t="n">
         <v>140</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="s">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="D71" t="n">
+      <c r="D71" s="0" t="n">
         <v>130</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="s">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="D72" t="n">
+      <c r="D72" s="0" t="n">
         <v>27890</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="s">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="D73" t="n">
+      <c r="D73" s="0" t="n">
         <v>21400</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" t="s">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="D74" t="n">
+      <c r="D74" s="0" t="n">
         <v>13730</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="s">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="D75" t="n">
+      <c r="D75" s="0" t="n">
         <v>11410</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="s">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="D76" t="n">
+      <c r="D76" s="0" t="n">
         <v>7460</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" t="s">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="D77" t="n">
+      <c r="D77" s="0" t="n">
         <v>4950</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="s">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="D78" t="n">
+      <c r="D78" s="0" t="n">
         <v>4680</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="s">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D79" t="n">
+      <c r="D79" s="0" t="n">
         <v>4570</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" t="s">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="D80" t="n">
+      <c r="D80" s="0" t="n">
         <v>4550</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" t="s">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="D81" t="n">
+      <c r="D81" s="0" t="n">
         <v>4300</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" t="s">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="D82" t="n">
+      <c r="D82" s="0" t="n">
         <v>3590</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" t="s">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="D83" t="n">
+      <c r="D83" s="0" t="n">
         <v>2280</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" t="s">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="D84" t="n">
+      <c r="D84" s="0" t="n">
         <v>1930</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" t="s">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="D85" t="n">
+      <c r="D85" s="0" t="n">
         <v>1380</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" t="s">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="D86" t="n">
+      <c r="D86" s="0" t="n">
         <v>1340</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" t="s">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="D87" t="n">
+      <c r="D87" s="0" t="n">
         <v>1250</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" t="s">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="D88" t="n">
+      <c r="D88" s="0" t="n">
         <v>1220</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" t="s">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="D89" t="n">
+      <c r="D89" s="0" t="n">
         <v>1170</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" t="s">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="D90" t="n">
+      <c r="D90" s="0" t="n">
         <v>1130</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" t="s">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="D91" t="n">
+      <c r="D91" s="0" t="n">
         <v>1090</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" t="s">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="D92" t="n">
+      <c r="D92" s="0" t="n">
         <v>4480</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" t="s">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="D93" t="n">
+      <c r="D93" s="0" t="n">
         <v>3570</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" t="s">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="D94" t="n">
+      <c r="D94" s="0" t="n">
         <v>1420</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" t="s">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="D95" t="n">
+      <c r="D95" s="0" t="n">
         <v>1420</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="s">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="D96" t="n">
+      <c r="D96" s="0" t="n">
         <v>1330</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" t="s">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D97" t="n">
+      <c r="D97" s="0" t="n">
         <v>1290</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" t="s">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="D98" t="n">
+      <c r="D98" s="0" t="n">
         <v>1220</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="s">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="D99" t="n">
+      <c r="D99" s="0" t="n">
         <v>1100</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" t="s">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="D100" t="n">
+      <c r="D100" s="0" t="n">
         <v>930</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" t="s">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="D101" t="n">
+      <c r="D101" s="0" t="n">
         <v>860</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" t="s">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D102" t="n">
+      <c r="D102" s="0" t="n">
         <v>1420</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" t="s">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D103" t="n">
+      <c r="D103" s="0" t="n">
         <v>850</v>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" t="s">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="D104" t="n">
+      <c r="D104" s="0" t="n">
         <v>680</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" t="s">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="D105" t="n">
+      <c r="D105" s="0" t="n">
         <v>660</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" t="s">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="D106" t="n">
+      <c r="D106" s="0" t="n">
         <v>610</v>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" t="s">
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="D107" t="n">
+      <c r="D107" s="0" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" t="s">
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="D108" t="n">
+      <c r="D108" s="0" t="n">
         <v>470</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" t="s">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D109" t="n">
+      <c r="D109" s="0" t="n">
         <v>460</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" t="s">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="D110" t="n">
+      <c r="D110" s="0" t="n">
         <v>460</v>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" t="s">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="D111" t="n">
+      <c r="D111" s="0" t="n">
         <v>360</v>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" t="s">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="D112" t="n">
+      <c r="D112" s="0" t="n">
         <v>11680</v>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" t="s">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="D113" t="n">
+      <c r="D113" s="0" t="n">
         <v>9980</v>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" t="s">
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="D114" t="n">
+      <c r="D114" s="0" t="n">
         <v>7990</v>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" t="s">
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="D115" t="n">
+      <c r="D115" s="0" t="n">
         <v>7350</v>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" t="s">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D116" t="n">
+      <c r="D116" s="0" t="n">
         <v>6570</v>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" t="s">
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="D117" t="n">
+      <c r="D117" s="0" t="n">
         <v>6190</v>
       </c>
     </row>
-    <row r="118">
-      <c r="A118" t="s">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="D118" t="n">
+      <c r="D118" s="0" t="n">
         <v>5510</v>
       </c>
     </row>
-    <row r="119">
-      <c r="A119" t="s">
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="D119" t="n">
+      <c r="D119" s="0" t="n">
         <v>4890</v>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" t="s">
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="D120" t="n">
+      <c r="D120" s="0" t="n">
         <v>4340</v>
       </c>
     </row>
-    <row r="121">
-      <c r="A121" t="s">
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="D121" t="n">
+      <c r="D121" s="0" t="n">
         <v>4080</v>
       </c>
     </row>
-    <row r="122">
-      <c r="A122" t="s">
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="D122" t="n">
+      <c r="D122" s="0" t="n">
         <v>4430</v>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" t="s">
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="D123" t="n">
+      <c r="D123" s="0" t="n">
         <v>2400</v>
       </c>
     </row>
-    <row r="124">
-      <c r="A124" t="s">
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="D124" t="n">
+      <c r="D124" s="0" t="n">
         <v>1980</v>
       </c>
     </row>
-    <row r="125">
-      <c r="A125" t="s">
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="D125" t="n">
+      <c r="D125" s="0" t="n">
         <v>1830</v>
       </c>
     </row>
-    <row r="126">
-      <c r="A126" t="s">
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D126" t="n">
+      <c r="D126" s="0" t="n">
         <v>1760</v>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" t="s">
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="D127" t="n">
+      <c r="D127" s="0" t="n">
         <v>1520</v>
       </c>
     </row>
-    <row r="128">
-      <c r="A128" t="s">
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="D128" t="n">
+      <c r="D128" s="0" t="n">
         <v>1320</v>
       </c>
     </row>
-    <row r="129">
-      <c r="A129" t="s">
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="D129" t="n">
+      <c r="D129" s="0" t="n">
         <v>1300</v>
       </c>
     </row>
-    <row r="130">
-      <c r="A130" t="s">
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D130" t="n">
+      <c r="D130" s="0" t="n">
         <v>1200</v>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" t="s">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="D131" t="n">
+      <c r="D131" s="0" t="n">
         <v>1070</v>
       </c>
     </row>
-    <row r="132">
-      <c r="A132" t="s">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="D132" t="n">
+      <c r="D132" s="0" t="n">
         <v>5230</v>
       </c>
     </row>
-    <row r="133">
-      <c r="A133" t="s">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="D133" t="n">
+      <c r="D133" s="0" t="n">
         <v>3110</v>
       </c>
     </row>
-    <row r="134">
-      <c r="A134" t="s">
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="D134" t="n">
+      <c r="D134" s="0" t="n">
         <v>2500</v>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" t="s">
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="D135" t="n">
+      <c r="D135" s="0" t="n">
         <v>1740</v>
       </c>
     </row>
-    <row r="136">
-      <c r="A136" t="s">
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C136" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D136" t="n">
+      <c r="D136" s="0" t="n">
         <v>1320</v>
       </c>
     </row>
-    <row r="137">
-      <c r="A137" t="s">
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D137" t="n">
+      <c r="D137" s="0" t="n">
         <v>1240</v>
       </c>
     </row>
-    <row r="138">
-      <c r="A138" t="s">
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C138" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D138" t="n">
+      <c r="D138" s="0" t="n">
         <v>1190</v>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" t="s">
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="D139" t="n">
+      <c r="D139" s="0" t="n">
         <v>1180</v>
       </c>
     </row>
-    <row r="140">
-      <c r="A140" t="s">
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="D140" t="n">
+      <c r="D140" s="0" t="n">
         <v>1080</v>
       </c>
     </row>
-    <row r="141">
-      <c r="A141" t="s">
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C141" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="D141" t="n">
+      <c r="D141" s="0" t="n">
         <v>1060</v>
       </c>
     </row>
-    <row r="142">
-      <c r="A142" t="s">
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C142" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="D142" t="n">
+      <c r="D142" s="0" t="n">
         <v>22810</v>
       </c>
     </row>
-    <row r="143">
-      <c r="A143" t="s">
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="D143" t="n">
+      <c r="D143" s="0" t="n">
         <v>20990</v>
       </c>
     </row>
-    <row r="144">
-      <c r="A144" t="s">
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C144" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D144" t="n">
+      <c r="D144" s="0" t="n">
         <v>8670</v>
       </c>
     </row>
-    <row r="145">
-      <c r="A145" t="s">
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="D145" t="n">
+      <c r="D145" s="0" t="n">
         <v>7420</v>
       </c>
     </row>
-    <row r="146">
-      <c r="A146" t="s">
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="D146" t="n">
+      <c r="D146" s="0" t="n">
         <v>3110</v>
       </c>
     </row>
-    <row r="147">
-      <c r="A147" t="s">
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="D147" t="n">
+      <c r="D147" s="0" t="n">
         <v>2050</v>
       </c>
     </row>
-    <row r="148">
-      <c r="A148" t="s">
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C148" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="D148" t="n">
+      <c r="D148" s="0" t="n">
         <v>1530</v>
       </c>
     </row>
-    <row r="149">
-      <c r="A149" t="s">
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C149" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="D149" t="n">
+      <c r="D149" s="0" t="n">
         <v>1530</v>
       </c>
     </row>
-    <row r="150">
-      <c r="A150" t="s">
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D150" t="n">
+      <c r="D150" s="0" t="n">
         <v>1440</v>
       </c>
     </row>
-    <row r="151">
-      <c r="A151" t="s">
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C151" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="D151" t="n">
+      <c r="D151" s="0" t="n">
         <v>1050</v>
       </c>
     </row>
-    <row r="152">
-      <c r="A152" t="s">
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C152" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D152" t="n">
+      <c r="D152" s="0" t="n">
         <v>8940</v>
       </c>
     </row>
-    <row r="153">
-      <c r="A153" t="s">
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C153" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="D153" t="n">
+      <c r="D153" s="0" t="n">
         <v>3330</v>
       </c>
     </row>
-    <row r="154">
-      <c r="A154" t="s">
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C154" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="D154" t="n">
+      <c r="D154" s="0" t="n">
         <v>2330</v>
       </c>
     </row>
-    <row r="155">
-      <c r="A155" t="s">
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="D155" t="n">
+      <c r="D155" s="0" t="n">
         <v>1790</v>
       </c>
     </row>
-    <row r="156">
-      <c r="A156" t="s">
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C156" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="D156" t="n">
+      <c r="D156" s="0" t="n">
         <v>1790</v>
       </c>
     </row>
-    <row r="157">
-      <c r="A157" t="s">
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C157" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="D157" t="n">
+      <c r="D157" s="0" t="n">
         <v>1720</v>
       </c>
     </row>
-    <row r="158">
-      <c r="A158" t="s">
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="D158" t="n">
+      <c r="D158" s="0" t="n">
         <v>1680</v>
       </c>
     </row>
-    <row r="159">
-      <c r="A159" t="s">
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="D159" t="n">
+      <c r="D159" s="0" t="n">
         <v>1550</v>
       </c>
     </row>
-    <row r="160">
-      <c r="A160" t="s">
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C160" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="D160" t="n">
+      <c r="D160" s="0" t="n">
         <v>1350</v>
       </c>
     </row>
-    <row r="161">
-      <c r="A161" t="s">
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="D161" t="n">
+      <c r="D161" s="0" t="n">
         <v>1260</v>
       </c>
     </row>
-    <row r="162">
-      <c r="A162" t="s">
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C162" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="D162" t="n">
+      <c r="D162" s="0" t="n">
         <v>450</v>
       </c>
     </row>
-    <row r="163">
-      <c r="A163" t="s">
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C163" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="D163" t="n">
+      <c r="D163" s="0" t="n">
         <v>440</v>
       </c>
     </row>
-    <row r="164">
-      <c r="A164" t="s">
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C164" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="D164" t="n">
+      <c r="D164" s="0" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="165">
-      <c r="A165" t="s">
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C165" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="D165" t="n">
+      <c r="D165" s="0" t="n">
         <v>290</v>
       </c>
     </row>
-    <row r="166">
-      <c r="A166" t="s">
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C166" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="D166" t="n">
+      <c r="D166" s="0" t="n">
         <v>260</v>
       </c>
     </row>
-    <row r="167">
-      <c r="A167" t="s">
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C167" s="0" t="s">
         <v>298</v>
       </c>
-      <c r="D167" t="n">
+      <c r="D167" s="0" t="n">
         <v>180</v>
       </c>
     </row>
-    <row r="168">
-      <c r="A168" t="s">
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C168" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="D168" t="n">
+      <c r="D168" s="0" t="n">
         <v>160</v>
       </c>
     </row>
-    <row r="169">
-      <c r="A169" t="s">
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="D169" t="n">
+      <c r="D169" s="0" t="n">
         <v>160</v>
       </c>
     </row>
-    <row r="170">
-      <c r="A170" t="s">
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C170" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="D170" t="n">
+      <c r="D170" s="0" t="n">
         <v>140</v>
       </c>
     </row>
-    <row r="171">
-      <c r="A171" t="s">
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C171" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D171" t="n">
+      <c r="D171" s="0" t="n">
         <v>140</v>
       </c>
     </row>
-    <row r="172">
-      <c r="A172" t="s">
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C172" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="D172" t="n">
+      <c r="D172" s="0" t="n">
         <v>5380</v>
       </c>
     </row>
-    <row r="173">
-      <c r="A173" t="s">
+    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B173" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C173" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="D173" t="n">
+      <c r="D173" s="0" t="n">
         <v>1730</v>
       </c>
     </row>
-    <row r="174">
-      <c r="A174" t="s">
+    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C174" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="D174" t="n">
+      <c r="D174" s="0" t="n">
         <v>1630</v>
       </c>
     </row>
-    <row r="175">
-      <c r="A175" t="s">
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C175" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="D175" t="n">
+      <c r="D175" s="0" t="n">
         <v>1510</v>
       </c>
     </row>
-    <row r="176">
-      <c r="A176" t="s">
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B176" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C176" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="D176" t="n">
+      <c r="D176" s="0" t="n">
         <v>1510</v>
       </c>
     </row>
-    <row r="177">
-      <c r="A177" t="s">
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C177" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="D177" t="n">
+      <c r="D177" s="0" t="n">
         <v>1210</v>
       </c>
     </row>
-    <row r="178">
-      <c r="A178" t="s">
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D178" t="n">
+      <c r="D178" s="0" t="n">
         <v>1190</v>
       </c>
     </row>
-    <row r="179">
-      <c r="A179" t="s">
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B179" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C179" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="D179" t="n">
+      <c r="D179" s="0" t="n">
         <v>1010</v>
       </c>
     </row>
-    <row r="180">
-      <c r="A180" t="s">
+    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D180" t="n">
+      <c r="D180" s="0" t="n">
         <v>810</v>
       </c>
     </row>
-    <row r="181">
-      <c r="A181" t="s">
+    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C181" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D181" t="n">
+      <c r="D181" s="0" t="n">
         <v>690</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>